<commit_message>
jenkins file added for selenium grid
</commit_message>
<xml_diff>
--- a/target/test-classes/excel/testdata.xlsx
+++ b/target/test-classes/excel/testdata.xlsx
@@ -528,7 +528,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -594,7 +594,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>

</xml_diff>